<commit_message>
URL update to admin for all apis
</commit_message>
<xml_diff>
--- a/Admin APIs.xlsx
+++ b/Admin APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NitsKundanProject\psm_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{953488D9-0B08-4415-84DA-7DB05E8C5CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53997902-5DCC-4DBF-ABC7-287DD9CF4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15492D3B-614E-45E1-80E6-0CAC308F0F89}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Module</t>
   </si>
   <si>
-    <t>/api/district/get-single-distric</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
@@ -64,18 +61,12 @@
     <t>District</t>
   </si>
   <si>
-    <t>/api/district/districts</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
     <t>{
   "name": "Nagpur"
 }</t>
-  </si>
-  <si>
-    <t>/api/district/districts_ddl</t>
   </si>
   <si>
     <t>Comments</t>
@@ -93,18 +84,12 @@
     <t>this is use for all district on listing page</t>
   </si>
   <si>
-    <t>/api/district/delete-district</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
     <t>{
   "id": 33
 }</t>
-  </si>
-  <si>
-    <t>/api/district/update-district</t>
   </si>
   <si>
     <t>PUT</t>
@@ -114,21 +99,6 @@
   "id": 22,
   "name": "Nagpur"
 }</t>
-  </si>
-  <si>
-    <t>/api/taluka/get-single-taluka</t>
-  </si>
-  <si>
-    <t>/api/taluka/talukas</t>
-  </si>
-  <si>
-    <t>/api/taluka/create-taluka</t>
-  </si>
-  <si>
-    <t>/api/taluka/delete-taluka</t>
-  </si>
-  <si>
-    <t>/api/taluka/update-taluka</t>
   </si>
   <si>
     <t>UPDATE</t>
@@ -148,21 +118,6 @@
   "district_id": 22,
   "name": "Aajni"
 }</t>
-  </si>
-  <si>
-    <t>/api/gram-panchayat/get-single-gram-panchayat</t>
-  </si>
-  <si>
-    <t>/api/gram-panchayat/all-gram-panchayat</t>
-  </si>
-  <si>
-    <t>/api/gram-panchayat/create-gram-panchayat</t>
-  </si>
-  <si>
-    <t>/api/gram-panchayat/delete-gram-panchayat</t>
-  </si>
-  <si>
-    <t>/api/gram-panchayat/update-gram-panchayat</t>
   </si>
   <si>
     <t>Gram Panchayat</t>
@@ -181,6 +136,51 @@
   "taluka_id": 1,
   "name": "Aajni"
 }</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-distric</t>
+  </si>
+  <si>
+    <t>/api/admin/districts</t>
+  </si>
+  <si>
+    <t>/api/admin/districts_ddl</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-district</t>
+  </si>
+  <si>
+    <t>/api/admin/update-district</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-taluka</t>
+  </si>
+  <si>
+    <t>/api/admin/talukas</t>
+  </si>
+  <si>
+    <t>/api/admin/create-taluka</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-taluka</t>
+  </si>
+  <si>
+    <t>/api/admin/update-taluka</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-gram-panchayat</t>
+  </si>
+  <si>
+    <t>/api/admin/all-gram-panchayat</t>
+  </si>
+  <si>
+    <t>/api/admin/create-gram-panchayat</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-gram-panchayat</t>
+  </si>
+  <si>
+    <t>/api/admin/update-gram-panchayat</t>
   </si>
 </sst>
 </file>
@@ -247,6 +247,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -255,9 +258,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,12 +602,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A7"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="40.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="5"/>
     <col min="4" max="4" width="45.21875" customWidth="1"/>
@@ -628,210 +628,210 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4" t="s">
+      <c r="D19" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update crud on gat grampanchayat
</commit_message>
<xml_diff>
--- a/Admin APIs.xlsx
+++ b/Admin APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NitsKundanProject\psm_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53997902-5DCC-4DBF-ABC7-287DD9CF4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69A819E-4000-4CEC-8738-71A30997C9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15492D3B-614E-45E1-80E6-0CAC308F0F89}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>URL</t>
   </si>
@@ -181,6 +181,79 @@
   </si>
   <si>
     <t>/api/admin/update-gram-panchayat</t>
+  </si>
+  <si>
+    <t>/api/admin/get-taluka-list-by-distict-id</t>
+  </si>
+  <si>
+    <t>{
+  "district_id": 23
+}</t>
+  </si>
+  <si>
+    <t>It is used for when we select the district then show all the taluka list</t>
+  </si>
+  <si>
+    <t>/api/admin/create-gat-gram-panchayat</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-gat-gram-panchaya</t>
+  </si>
+  <si>
+    <t>{
+  "district_id": 22,
+  "taluka_id": 1,
+  "grampanchayat_id": 3,
+  "name": "Borda gat"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "pageNumber": 1,
+  "searchText": ""
+}</t>
+  </si>
+  <si>
+    <t>Gat Gram Panchayat</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-gat-gram-panchayat</t>
+  </si>
+  <si>
+    <t>{
+  "id": 4
+}</t>
+  </si>
+  <si>
+    <t>/api/admin/get-grampanchayat-list-by-taluka-id</t>
+  </si>
+  <si>
+    <t>/api/admin/update-gat-gram-panchayat</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-gat-gram-panchayat</t>
+  </si>
+  <si>
+    <t>it is used for when select taluka then show all the gram panchayat list</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "district_id": 22,
+  "taluka_id": 1,
+  "grampanchayat_id": 1,
+  "name": "Aajni"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 8
+}</t>
+  </si>
+  <si>
+    <t>{
+  "taluka_id": 1
+}</t>
   </si>
 </sst>
 </file>
@@ -230,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -258,6 +331,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,11 +677,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37EACC-0ADA-46A9-ACAF-241202A156F4}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,7 +690,7 @@
     <col min="2" max="2" width="40.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="5"/>
     <col min="4" max="4" width="45.21875" customWidth="1"/>
-    <col min="5" max="5" width="50" customWidth="1"/>
+    <col min="5" max="5" width="50" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -627,7 +706,7 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -665,7 +744,7 @@
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -680,7 +759,7 @@
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -798,7 +877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="4" t="s">
         <v>36</v>
@@ -810,7 +889,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="4" t="s">
         <v>37</v>
@@ -822,7 +901,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="4" t="s">
         <v>38</v>
@@ -834,8 +913,102 @@
         <v>23</v>
       </c>
     </row>
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A21:XFD21"/>
+    <mergeCell ref="A22:A27"/>
     <mergeCell ref="A8:XFD8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A2:A7"/>

</xml_diff>

<commit_message>
update floor, prakar, malmatehce prakar, users
</commit_message>
<xml_diff>
--- a/Admin APIs.xlsx
+++ b/Admin APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NitsKundanProject\psm_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69A819E-4000-4CEC-8738-71A30997C9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589A73C3-6284-41BE-AF1E-E6962A4592AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15492D3B-614E-45E1-80E6-0CAC308F0F89}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
   <si>
     <t>URL</t>
   </si>
@@ -253,6 +253,155 @@
   <si>
     <t>{
   "taluka_id": 1
+}</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>/api/user/create-new-user</t>
+  </si>
+  <si>
+    <t>/api/user/update-user</t>
+  </si>
+  <si>
+    <t>/api/user/users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/user/get-signle-user/1 </t>
+  </si>
+  <si>
+    <t>/api/user/delete-signle-user/1</t>
+  </si>
+  <si>
+    <t>/api/user/login</t>
+  </si>
+  <si>
+    <t>{
+  "district_id": 22,
+  "taluka_id": 1,
+  "grampanchayat_id": 1,
+  "gatgrampanchayat_id": 1,
+  "name": "Kundan M Kotangale",
+  "email": "kundanmkotangale@gmail.com",
+  "username": "Kundan1993",
+  "pwd": "Test@123"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "district_id": 22,
+  "taluka_id": 1,
+  "grampanchayat_id": 1,
+  "gatgrampanchayat_id": 1,
+  "name": "Kundan M Kotangale",
+  "email": "kundanmkotangale@gmail.com",
+  "username": "Kundan93"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "username": "admin",
+  "password": "admin@123"
+}</t>
+  </si>
+  <si>
+    <t>/api/admin/get-gat-grampanchayat-list-by-grampanchayat-id</t>
+  </si>
+  <si>
+    <t>{
+  "grampanchayat_id": 1
+}</t>
+  </si>
+  <si>
+    <t>When we select gram panchayat from drop doen then in gat grampanchayat list will dislay all list</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>/api/admin/create-floor</t>
+  </si>
+  <si>
+    <t>/api/admin/update-floor</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-floors</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-floor/1</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-floor/1</t>
+  </si>
+  <si>
+    <t>{
+  "floor_name": "Third Floor"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "floor_name": "Ground Floor"
+}</t>
+  </si>
+  <si>
+    <t>/api/admin/create-prakar</t>
+  </si>
+  <si>
+    <t>/api/admin/update-prakar</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-prakars</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-prakar/1</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-prakar/1</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "prakar_name": "Gavthan"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "prakar_name": "Gavthan"
+}</t>
+  </si>
+  <si>
+    <t>Prakar</t>
+  </si>
+  <si>
+    <t>Malmatteche Prakar</t>
+  </si>
+  <si>
+    <t>/api/admin/create-malmatteche-prakar</t>
+  </si>
+  <si>
+    <t>/api/admin/update-malmatteche-prakar</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-malmatteche-prakars</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-malmatteche-prakar/1</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-malmatteche-prakar/1</t>
+  </si>
+  <si>
+    <t>{
+  "name": "Nivashi"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "name": "Nivashi"
 }</t>
   </si>
 </sst>
@@ -323,8 +472,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -332,11 +484,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,20 +826,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37EACC-0ADA-46A9-ACAF-241202A156F4}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="40.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="5"/>
     <col min="4" max="4" width="45.21875" customWidth="1"/>
-    <col min="5" max="5" width="50" style="11" customWidth="1"/>
+    <col min="5" max="5" width="50" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -706,12 +855,12 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -725,7 +874,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -737,19 +886,19 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
@@ -759,12 +908,12 @@
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
@@ -776,7 +925,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
@@ -787,9 +936,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -803,7 +952,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
@@ -815,7 +964,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
@@ -827,7 +976,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
@@ -839,7 +988,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
@@ -850,9 +999,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -866,7 +1015,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
@@ -878,7 +1027,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
@@ -890,7 +1039,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
@@ -902,7 +1051,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
@@ -923,13 +1072,13 @@
       <c r="D20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -943,7 +1092,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="4" t="s">
         <v>43</v>
       </c>
@@ -955,7 +1104,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
@@ -967,7 +1116,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="4" t="s">
         <v>50</v>
       </c>
@@ -979,7 +1128,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="4" t="s">
         <v>51</v>
       </c>
@@ -991,7 +1140,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="4" t="s">
         <v>49</v>
       </c>
@@ -1001,12 +1150,270 @@
       <c r="D27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="8" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="28" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="9"/>
+      <c r="B38" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="9"/>
+      <c r="B40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="9"/>
+      <c r="B44" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="9"/>
+      <c r="B45" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="9"/>
+      <c r="B46" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="9"/>
+      <c r="B47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="10"/>
+      <c r="B50" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="10"/>
+      <c r="B51" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="10"/>
+      <c r="B53" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="15">
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A48:XFD48"/>
+    <mergeCell ref="A49:A53"/>
     <mergeCell ref="A21:XFD21"/>
     <mergeCell ref="A22:A27"/>
     <mergeCell ref="A8:XFD8"/>
@@ -1014,7 +1421,13 @@
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A14:XFD14"/>
     <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A28:XFD28"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A36:XFD36"/>
+    <mergeCell ref="A42:XFD42"/>
+    <mergeCell ref="A37:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
malmatta crud operation done
</commit_message>
<xml_diff>
--- a/Admin APIs.xlsx
+++ b/Admin APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NitsKundanProject\psm_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589A73C3-6284-41BE-AF1E-E6962A4592AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3712960-092F-4660-8436-1F82F24ACA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15492D3B-614E-45E1-80E6-0CAC308F0F89}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="111">
   <si>
     <t>URL</t>
   </si>
@@ -402,6 +402,74 @@
     <t>{
   "id": 1,
   "name": "Nivashi"
+}</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-malmatteche-prakar-ddl-list</t>
+  </si>
+  <si>
+    <t>/api/admin/create-milkat-vapar</t>
+  </si>
+  <si>
+    <t>/api/admin/update-milkat-vapar</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-milkat-vapar</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-milkat-vapar/3</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-milkat-vapar/3</t>
+  </si>
+  <si>
+    <t>{
+  "malmatteche_prakar_id": 1,
+  "name": "Society"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 2,
+  "malmatteche_prakar_id": 1,
+  "name": "Society"
+}</t>
+  </si>
+  <si>
+    <t>Milkat Vapar</t>
+  </si>
+  <si>
+    <t>Malmatta</t>
+  </si>
+  <si>
+    <t>mal matteche prakar dropdown select 2</t>
+  </si>
+  <si>
+    <t>/api/admin/create-malmatta</t>
+  </si>
+  <si>
+    <t>/api/admin/update-malmatta</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-malmatta</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-malmatta/1</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-malmatta/1</t>
+  </si>
+  <si>
+    <t>{
+  "malmatteche_prakar_id": 1,
+  "milkateche_varnan": "Khula bhukhand"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "malmatteche_prakar_id": 1,
+  "milkateche_varnan": "Khula bhukhand"
 }</t>
   </si>
 </sst>
@@ -826,11 +894,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37EACC-0ADA-46A9-ACAF-241202A156F4}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,7 +1421,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>85</v>
       </c>
@@ -1367,7 +1435,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="4" t="s">
         <v>87</v>
@@ -1379,7 +1447,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="10"/>
       <c r="B51" s="4" t="s">
         <v>88</v>
@@ -1391,7 +1459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="4" t="s">
         <v>89</v>
@@ -1400,7 +1468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="4" t="s">
         <v>90</v>
@@ -1409,18 +1477,148 @@
         <v>13</v>
       </c>
     </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+      <c r="B54" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A63" s="9"/>
+      <c r="B63" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="9"/>
+      <c r="B64" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="9"/>
+      <c r="B65" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="9"/>
+      <c r="B66" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="A48:XFD48"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A21:XFD21"/>
-    <mergeCell ref="A22:A27"/>
+  <mergeCells count="19">
+    <mergeCell ref="A55:XFD55"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="A61:XFD61"/>
+    <mergeCell ref="A62:A66"/>
     <mergeCell ref="A8:XFD8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A14:XFD14"/>
     <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A48:XFD48"/>
+    <mergeCell ref="A21:XFD21"/>
+    <mergeCell ref="A22:A27"/>
     <mergeCell ref="A28:XFD28"/>
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="A36:XFD36"/>

</xml_diff>

<commit_message>
update tax crud operations
</commit_message>
<xml_diff>
--- a/Admin APIs.xlsx
+++ b/Admin APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NitsKundanProject\psm_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3712960-092F-4660-8436-1F82F24ACA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFA3635-CBEE-42F6-8732-DA9F08F0D156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15492D3B-614E-45E1-80E6-0CAC308F0F89}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="119">
   <si>
     <t>URL</t>
   </si>
@@ -470,6 +470,35 @@
   "id": 1,
   "malmatteche_prakar_id": 1,
   "milkateche_varnan": "Khula bhukhand"
+}</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>/api/admin/create-tax</t>
+  </si>
+  <si>
+    <t>/api/admin/update-tax</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-tax</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-tax/1</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-tax/1</t>
+  </si>
+  <si>
+    <t>{
+  "tax_name": "Electric"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id":2,
+  "tax_name": "Electric"
 }</t>
   </si>
 </sst>
@@ -494,7 +523,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,6 +533,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -552,7 +587,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -894,11 +932,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37EACC-0ADA-46A9-ACAF-241202A156F4}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1004,7 +1042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>18</v>
@@ -1067,7 +1105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>21</v>
@@ -1144,7 +1182,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>46</v>
@@ -1222,7 +1260,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>56</v>
@@ -1306,7 +1344,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>69</v>
@@ -1363,7 +1401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>84</v>
@@ -1420,7 +1458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>85</v>
@@ -1489,7 +1527,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
         <v>101</v>
@@ -1546,7 +1584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>102</v>
@@ -1585,7 +1623,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="9"/>
       <c r="B65" s="4" t="s">
         <v>107</v>
@@ -1594,7 +1632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
       <c r="B66" s="4" t="s">
         <v>108</v>
@@ -1603,18 +1641,69 @@
         <v>13</v>
       </c>
     </row>
+    <row r="67" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="9"/>
+      <c r="B69" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="9"/>
+      <c r="B70" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="9"/>
+      <c r="B71" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="9"/>
+      <c r="B72" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A55:XFD55"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="A61:XFD61"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="A8:XFD8"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A14:XFD14"/>
-    <mergeCell ref="A15:A19"/>
+  <mergeCells count="22">
+    <mergeCell ref="A67:XFD67"/>
+    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="A73:XFD73"/>
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A48:XFD48"/>
     <mergeCell ref="A21:XFD21"/>
@@ -1624,6 +1713,16 @@
     <mergeCell ref="A36:XFD36"/>
     <mergeCell ref="A42:XFD42"/>
     <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A8:XFD8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A14:XFD14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A55:XFD55"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="A61:XFD61"/>
+    <mergeCell ref="A62:A66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
done other tax details
</commit_message>
<xml_diff>
--- a/Admin APIs.xlsx
+++ b/Admin APIs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NitsKundanProject\psm_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFA3635-CBEE-42F6-8732-DA9F08F0D156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FB596C-AEA0-4CFF-A1E4-3DDF141A4C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15492D3B-614E-45E1-80E6-0CAC308F0F89}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="129">
   <si>
     <t>URL</t>
   </si>
@@ -499,6 +499,74 @@
     <t>{
   "id":2,
   "tax_name": "Electric"
+}</t>
+  </si>
+  <si>
+    <t>Other Tax</t>
+  </si>
+  <si>
+    <t>/api/admin/api/admin/create-other-tax</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-tax-details</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-complete-other-tax/2</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-other-tax/2</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-other-tax</t>
+  </si>
+  <si>
+    <t>/api/admin/update-other-tax</t>
+  </si>
+  <si>
+    <t>{
+  "district_id": 22,
+  "taluka_id": 1,
+  "grampanchayat_id": 5,
+  "tax_details_config": [
+    {
+      "id": 1,
+      "label": "विजकर व दिवाबत्ती कर",
+      "rate": 20,
+      "is_active": 0
+    },
+    {
+      "id": 2,
+      "label": "सफाई करकर",
+      "rate": 25,
+      "is_active": 0
+    }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 2,
+  "district_id": 22,
+  "taluka_id": 1,
+  "grampanchayat_id": 4,
+  "tax_details_config": [
+    {
+      "id": 1,
+      "label": "विजकर व दिवाबत्ती कर",
+      "rate": 28
+    },
+    {
+      "id": 2,
+      "label": "सफाई करकर",
+      "rate": 30
+    }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "tax_details_config": 1
 }</t>
   </si>
 </sst>
@@ -581,14 +649,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -932,11 +1000,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37EACC-0ADA-46A9-ACAF-241202A156F4}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,7 +1034,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -980,7 +1048,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -992,7 +1060,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
@@ -1004,7 +1072,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
@@ -1019,7 +1087,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1031,7 +1099,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
@@ -1044,7 +1112,7 @@
     </row>
     <row r="8" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1058,7 +1126,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
@@ -1070,7 +1138,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
@@ -1082,7 +1150,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
@@ -1094,7 +1162,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
@@ -1107,7 +1175,7 @@
     </row>
     <row r="14" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1121,7 +1189,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1133,7 +1201,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
@@ -1145,7 +1213,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
@@ -1157,7 +1225,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
@@ -1182,9 +1250,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1198,7 +1266,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="4" t="s">
         <v>43</v>
       </c>
@@ -1210,7 +1278,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
@@ -1222,7 +1290,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="4" t="s">
         <v>50</v>
       </c>
@@ -1234,7 +1302,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="4" t="s">
         <v>51</v>
       </c>
@@ -1246,7 +1314,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="4" t="s">
         <v>49</v>
       </c>
@@ -1260,9 +1328,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:5" ht="144" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1276,7 +1344,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="144" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="4" t="s">
         <v>58</v>
       </c>
@@ -1288,7 +1356,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="4" t="s">
         <v>59</v>
       </c>
@@ -1300,7 +1368,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="4" t="s">
         <v>60</v>
       </c>
@@ -1309,7 +1377,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="4" t="s">
         <v>61</v>
       </c>
@@ -1318,7 +1386,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="4" t="s">
         <v>62</v>
       </c>
@@ -1330,7 +1398,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="4" t="s">
         <v>66</v>
       </c>
@@ -1344,9 +1412,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -1360,7 +1428,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="4" t="s">
         <v>71</v>
       </c>
@@ -1372,7 +1440,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="4" t="s">
         <v>72</v>
       </c>
@@ -1384,7 +1452,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="4" t="s">
         <v>73</v>
       </c>
@@ -1393,7 +1461,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="4" t="s">
         <v>74</v>
       </c>
@@ -1401,9 +1469,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -1417,7 +1485,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="4" t="s">
         <v>78</v>
       </c>
@@ -1429,7 +1497,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="4" t="s">
         <v>79</v>
       </c>
@@ -1441,7 +1509,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="4" t="s">
         <v>80</v>
       </c>
@@ -1450,7 +1518,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="4" t="s">
         <v>81</v>
       </c>
@@ -1458,9 +1526,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -1474,7 +1542,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="4" t="s">
         <v>87</v>
       </c>
@@ -1486,7 +1554,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="4" t="s">
         <v>88</v>
       </c>
@@ -1498,7 +1566,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="10"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="4" t="s">
         <v>89</v>
       </c>
@@ -1507,7 +1575,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="4" t="s">
         <v>90</v>
       </c>
@@ -1516,7 +1584,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="10"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="4" t="s">
         <v>93</v>
       </c>
@@ -1527,9 +1595,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="10" t="s">
         <v>101</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -1543,7 +1611,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
+      <c r="A57" s="10"/>
       <c r="B57" s="4" t="s">
         <v>95</v>
       </c>
@@ -1555,7 +1623,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="9"/>
+      <c r="A58" s="10"/>
       <c r="B58" s="4" t="s">
         <v>96</v>
       </c>
@@ -1567,7 +1635,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
+      <c r="A59" s="10"/>
       <c r="B59" s="4" t="s">
         <v>97</v>
       </c>
@@ -1576,7 +1644,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
+      <c r="A60" s="10"/>
       <c r="B60" s="4" t="s">
         <v>98</v>
       </c>
@@ -1584,9 +1652,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="10" t="s">
         <v>102</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -1600,7 +1668,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A63" s="9"/>
+      <c r="A63" s="10"/>
       <c r="B63" s="4" t="s">
         <v>105</v>
       </c>
@@ -1612,7 +1680,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="9"/>
+      <c r="A64" s="10"/>
       <c r="B64" s="4" t="s">
         <v>106</v>
       </c>
@@ -1624,7 +1692,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="9"/>
+      <c r="A65" s="10"/>
       <c r="B65" s="4" t="s">
         <v>107</v>
       </c>
@@ -1633,7 +1701,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
+      <c r="A66" s="10"/>
       <c r="B66" s="4" t="s">
         <v>108</v>
       </c>
@@ -1641,9 +1709,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="68" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="10" t="s">
         <v>111</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -1657,7 +1725,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
+      <c r="A69" s="10"/>
       <c r="B69" s="4" t="s">
         <v>113</v>
       </c>
@@ -1669,7 +1737,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="9"/>
+      <c r="A70" s="10"/>
       <c r="B70" s="4" t="s">
         <v>114</v>
       </c>
@@ -1681,7 +1749,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="9"/>
+      <c r="A71" s="10"/>
       <c r="B71" s="4" t="s">
         <v>115</v>
       </c>
@@ -1690,7 +1758,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="9"/>
+      <c r="A72" s="10"/>
       <c r="B72" s="4" t="s">
         <v>116</v>
       </c>
@@ -1698,19 +1766,80 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A74" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="10"/>
+      <c r="B75" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="10"/>
+      <c r="B76" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="10"/>
+      <c r="B77" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="10"/>
+      <c r="B78" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="10"/>
+      <c r="B79" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A67:XFD67"/>
-    <mergeCell ref="A68:A72"/>
-    <mergeCell ref="A73:XFD73"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="A48:XFD48"/>
-    <mergeCell ref="A21:XFD21"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="A28:XFD28"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A36:XFD36"/>
+  <mergeCells count="24">
+    <mergeCell ref="A74:A79"/>
+    <mergeCell ref="A80:XFD80"/>
     <mergeCell ref="A42:XFD42"/>
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A8:XFD8"/>
@@ -1718,6 +1847,16 @@
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A14:XFD14"/>
     <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A21:XFD21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A28:XFD28"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A36:XFD36"/>
+    <mergeCell ref="A67:XFD67"/>
+    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="A73:XFD73"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A48:XFD48"/>
     <mergeCell ref="A55:XFD55"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="A56:A60"/>

</xml_diff>

<commit_message>
done annual tax API
</commit_message>
<xml_diff>
--- a/Admin APIs.xlsx
+++ b/Admin APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NitsKundanProject\psm_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FB596C-AEA0-4CFF-A1E4-3DDF141A4C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FBA934-F810-47D4-B8DC-7EAAF3D4AA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15492D3B-614E-45E1-80E6-0CAC308F0F89}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="138">
   <si>
     <t>URL</t>
   </si>
@@ -458,19 +458,6 @@
   </si>
   <si>
     <t>/api/admin/delete-malmatta/1</t>
-  </si>
-  <si>
-    <t>{
-  "malmatteche_prakar_id": 1,
-  "milkateche_varnan": "Khula bhukhand"
-}</t>
-  </si>
-  <si>
-    <t>{
-  "id": 1,
-  "malmatteche_prakar_id": 1,
-  "milkateche_varnan": "Khula bhukhand"
-}</t>
   </si>
   <si>
     <t>Tax</t>
@@ -568,6 +555,59 @@
   "id": 1,
   "tax_details_config": 1
 }</t>
+  </si>
+  <si>
+    <t>{
+  "milkateche_varnan": "लोडबारिंग आर सी सी बंगला",
+  "malmatteche_prakar_name": "आर सी सी"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "malmatteche_prakar_name": "कच्चे",
+  "milkateche_varnan": "वीटा, कवेलु, सीमेंट"
+}</t>
+  </si>
+  <si>
+    <t>Annual Tax</t>
+  </si>
+  <si>
+    <t>/api/admin/api/admin/create-annual-tax</t>
+  </si>
+  <si>
+    <t>{
+  "district_id": 1,
+  "taluka_id": 2,
+  "grampanchayat_id": 1,
+  "gat_grampanchayat_id":1,
+  "malmatteche_prakar_id": 1,
+  "malmatteche_varnan_id": 1,
+  "annual_rate": 1400,
+  "aakarani_dar": 1.20
+}</t>
+  </si>
+  <si>
+    <t>/api/admin/update-annual-tax-rates</t>
+  </si>
+  <si>
+    <t>{
+  "id": 1,
+  "annual_rate": 1200,
+  "aakarani_dar": 5.5
+}</t>
+  </si>
+  <si>
+    <t>/api/admin/get-all-annual-tax</t>
+  </si>
+  <si>
+    <t>/api/admin/get-single-annual-tax/6</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-complete-annual-tax/6</t>
+  </si>
+  <si>
+    <t>/api/admin/delete-annual-tax-rates/1</t>
   </si>
 </sst>
 </file>
@@ -649,17 +689,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,11 +1040,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37EACC-0ADA-46A9-ACAF-241202A156F4}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80:XFD80"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,7 +1074,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1048,7 +1088,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1060,7 +1100,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
@@ -1072,7 +1112,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
@@ -1087,7 +1127,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1099,7 +1139,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
@@ -1110,9 +1150,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1126,7 +1166,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
@@ -1138,7 +1178,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
@@ -1150,7 +1190,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
@@ -1162,7 +1202,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
@@ -1173,9 +1213,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1189,7 +1229,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1201,7 +1241,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
@@ -1213,7 +1253,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
@@ -1225,7 +1265,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
@@ -1250,9 +1290,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1266,7 +1306,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="4" t="s">
         <v>43</v>
       </c>
@@ -1278,7 +1318,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
@@ -1290,7 +1330,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="4" t="s">
         <v>50</v>
       </c>
@@ -1302,7 +1342,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="4" t="s">
         <v>51</v>
       </c>
@@ -1314,7 +1354,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="4" t="s">
         <v>49</v>
       </c>
@@ -1328,9 +1368,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:5" ht="144" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1344,7 +1384,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="144" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="4" t="s">
         <v>58</v>
       </c>
@@ -1356,7 +1396,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="4" t="s">
         <v>59</v>
       </c>
@@ -1368,7 +1408,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="4" t="s">
         <v>60</v>
       </c>
@@ -1377,7 +1417,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="4" t="s">
         <v>61</v>
       </c>
@@ -1386,7 +1426,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="4" t="s">
         <v>62</v>
       </c>
@@ -1398,7 +1438,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="4" t="s">
         <v>66</v>
       </c>
@@ -1412,9 +1452,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="9" t="s">
         <v>69</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -1428,7 +1468,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="4" t="s">
         <v>71</v>
       </c>
@@ -1440,7 +1480,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="4" t="s">
         <v>72</v>
       </c>
@@ -1452,7 +1492,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="4" t="s">
         <v>73</v>
       </c>
@@ -1461,7 +1501,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="4" t="s">
         <v>74</v>
       </c>
@@ -1469,9 +1509,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
         <v>84</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -1485,7 +1525,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="4" t="s">
         <v>78</v>
       </c>
@@ -1497,7 +1537,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="4" t="s">
         <v>79</v>
       </c>
@@ -1509,7 +1549,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="4" t="s">
         <v>80</v>
       </c>
@@ -1518,7 +1558,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="4" t="s">
         <v>81</v>
       </c>
@@ -1526,9 +1566,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="12" t="s">
         <v>85</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -1542,7 +1582,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="11"/>
+      <c r="A50" s="12"/>
       <c r="B50" s="4" t="s">
         <v>87</v>
       </c>
@@ -1554,7 +1594,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="11"/>
+      <c r="A51" s="12"/>
       <c r="B51" s="4" t="s">
         <v>88</v>
       </c>
@@ -1566,7 +1606,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="11"/>
+      <c r="A52" s="12"/>
       <c r="B52" s="4" t="s">
         <v>89</v>
       </c>
@@ -1575,7 +1615,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="11"/>
+      <c r="A53" s="12"/>
       <c r="B53" s="4" t="s">
         <v>90</v>
       </c>
@@ -1584,7 +1624,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="11"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="4" t="s">
         <v>93</v>
       </c>
@@ -1595,9 +1635,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -1611,7 +1651,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A57" s="10"/>
+      <c r="A57" s="9"/>
       <c r="B57" s="4" t="s">
         <v>95</v>
       </c>
@@ -1623,7 +1663,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
+      <c r="A58" s="9"/>
       <c r="B58" s="4" t="s">
         <v>96</v>
       </c>
@@ -1635,7 +1675,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="10"/>
+      <c r="A59" s="9"/>
       <c r="B59" s="4" t="s">
         <v>97</v>
       </c>
@@ -1644,7 +1684,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="10"/>
+      <c r="A60" s="9"/>
       <c r="B60" s="4" t="s">
         <v>98</v>
       </c>
@@ -1652,9 +1692,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -1664,11 +1704,11 @@
         <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A63" s="10"/>
+      <c r="A63" s="9"/>
       <c r="B63" s="4" t="s">
         <v>105</v>
       </c>
@@ -1676,11 +1716,11 @@
         <v>15</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="10"/>
+      <c r="A64" s="9"/>
       <c r="B64" s="4" t="s">
         <v>106</v>
       </c>
@@ -1692,7 +1732,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="10"/>
+      <c r="A65" s="9"/>
       <c r="B65" s="4" t="s">
         <v>107</v>
       </c>
@@ -1701,7 +1741,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="10"/>
+      <c r="A66" s="9"/>
       <c r="B66" s="4" t="s">
         <v>108</v>
       </c>
@@ -1709,37 +1749,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="68" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="9"/>
+      <c r="B69" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="10"/>
-      <c r="B69" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="10"/>
+      <c r="A70" s="9"/>
       <c r="B70" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>7</v>
@@ -1749,54 +1789,54 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="10"/>
+      <c r="A71" s="9"/>
       <c r="B71" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="10"/>
+      <c r="A72" s="9"/>
       <c r="B72" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="74" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A74" s="10" t="s">
-        <v>119</v>
+      <c r="A74" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="10"/>
+      <c r="A75" s="9"/>
       <c r="B75" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="10"/>
+      <c r="A76" s="9"/>
       <c r="B76" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>7</v>
@@ -1806,49 +1846,109 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="10"/>
+      <c r="A77" s="9"/>
       <c r="B77" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="10"/>
+      <c r="A78" s="9"/>
       <c r="B78" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="10"/>
+      <c r="A79" s="9"/>
       <c r="B79" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A82" s="9"/>
+      <c r="B82" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="9"/>
+      <c r="B83" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="9"/>
+      <c r="B84" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="9"/>
+      <c r="B85" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B86" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="A81:A85"/>
     <mergeCell ref="A74:A79"/>
     <mergeCell ref="A80:XFD80"/>
     <mergeCell ref="A42:XFD42"/>
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A8:XFD8"/>
     <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A14:XFD14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A21:XFD21"/>
-    <mergeCell ref="A22:A27"/>
     <mergeCell ref="A28:XFD28"/>
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="A36:XFD36"/>
@@ -1862,6 +1962,11 @@
     <mergeCell ref="A56:A60"/>
     <mergeCell ref="A61:XFD61"/>
     <mergeCell ref="A62:A66"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A14:XFD14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A21:XFD21"/>
+    <mergeCell ref="A22:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>